<commit_message>
completed 5b, which is a little more flexible
</commit_message>
<xml_diff>
--- a/assignment_data_5b.xlsx
+++ b/assignment_data_5b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\next-best-position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94CBD04-B57C-45D1-80C6-C2DB20814279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDB6D9A-E691-4631-90C4-7F8B6264539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{1B66F183-0BCD-4F97-8FF8-4BD92C1308AE}"/>
   </bookViews>
@@ -80,12 +80,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,9 +130,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,9 +1498,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359C2FAD-099F-46C8-A0D9-E07FF297F409}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1468,9 +1510,9 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1482,114 +1524,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6032</v>
       </c>
-      <c r="B2" s="1">
-        <v>45538</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="8">
+        <v>45575</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6016</v>
       </c>
-      <c r="B3" s="1">
-        <v>45480</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
+        <v>45498</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6037</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>45451</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6033</v>
       </c>
-      <c r="B5" s="1">
-        <v>45575</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="2">
+        <v>45538</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6013</v>
       </c>
-      <c r="B6" s="1">
-        <v>45498</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>45480</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1891,7 +1920,7 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(1,180)</f>
-        <v>45549</v>
+        <v>45422</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1901,7 +1930,7 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45550</v>
+        <v>45598</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1911,7 +1940,7 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3" ca="1" si="0">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45729</v>
+        <v>45652</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1922,7 +1951,7 @@
       </c>
       <c r="F3" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45683</v>
+        <v>45467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>